<commit_message>
Se le dio formato a la documentación y se agregó crátula e índice Se controlaron todos los métodos y aquellos que no eran invocados fueron eliminados Se eliminaron todos los import innecesarios
</commit_message>
<xml_diff>
--- a/Documentación/1er Entrega Obligatorio DDA.xlsx
+++ b/Documentación/1er Entrega Obligatorio DDA.xlsx
@@ -376,7 +376,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -384,62 +384,86 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -742,104 +766,148 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B5:E11"/>
+  <dimension ref="A5:G13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="E11" sqref="B6:E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="11.5546875" style="1"/>
-    <col min="2" max="2" width="58.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.5546875" style="1" customWidth="1"/>
     <col min="3" max="3" width="13.109375" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17.88671875" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="16384" width="11.5546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="6" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="11" t="s">
+    <row r="5" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="17"/>
+      <c r="B5" s="17"/>
+      <c r="C5" s="17"/>
+      <c r="D5" s="17"/>
+      <c r="E5" s="17"/>
+      <c r="F5" s="17"/>
+      <c r="G5" s="17"/>
+    </row>
+    <row r="6" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="17"/>
+      <c r="B6" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="12" t="s">
+      <c r="C6" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="12" t="s">
+      <c r="D6" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="E6" s="13" t="s">
+      <c r="E6" s="20" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B7" s="8" t="s">
+      <c r="F6" s="17"/>
+      <c r="G6" s="17"/>
+    </row>
+    <row r="7" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A7" s="17"/>
+      <c r="B7" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="9" t="s">
+      <c r="C7" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="9" t="s">
+      <c r="D7" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="E7" s="10">
+      <c r="E7" s="23">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B8" s="3" t="s">
+      <c r="F7" s="17"/>
+      <c r="G7" s="17"/>
+    </row>
+    <row r="8" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A8" s="17"/>
+      <c r="B8" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="C8" s="2">
+      <c r="C8" s="25">
         <v>3</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D8" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="E8" s="4">
+      <c r="E8" s="26">
         <v>3</v>
       </c>
-    </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B9" s="3" t="s">
+      <c r="F8" s="17"/>
+      <c r="G8" s="17"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" s="17"/>
+      <c r="B9" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="C9" s="2">
+      <c r="C9" s="25">
         <v>16</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="D9" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="E9" s="4">
+      <c r="E9" s="26">
         <v>16</v>
       </c>
-    </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B10" s="3" t="s">
+      <c r="F9" s="17"/>
+      <c r="G9" s="17"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" s="17"/>
+      <c r="B10" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="C10" s="2">
+      <c r="C10" s="25">
         <v>1</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="D10" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="E10" s="4">
+      <c r="E10" s="26">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="5" t="s">
+      <c r="F10" s="17"/>
+      <c r="G10" s="17"/>
+    </row>
+    <row r="11" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="17"/>
+      <c r="B11" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="C11" s="6">
+      <c r="C11" s="28">
         <v>20</v>
       </c>
-      <c r="D11" s="6"/>
-      <c r="E11" s="7">
+      <c r="D11" s="28"/>
+      <c r="E11" s="29">
         <v>20</v>
       </c>
+      <c r="F11" s="17"/>
+      <c r="G11" s="17"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12" s="17"/>
+      <c r="B12" s="17"/>
+      <c r="C12" s="17"/>
+      <c r="D12" s="17"/>
+      <c r="E12" s="17"/>
+      <c r="F12" s="17"/>
+      <c r="G12" s="17"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13" s="17"/>
+      <c r="B13" s="17"/>
+      <c r="C13" s="17"/>
+      <c r="D13" s="17"/>
+      <c r="E13" s="17"/>
+      <c r="F13" s="17"/>
+      <c r="G13" s="17"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -851,8 +919,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:F27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16:E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -869,50 +937,50 @@
   <sheetData>
     <row r="2" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="3" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="18" t="s">
+      <c r="B3" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="19"/>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19"/>
-      <c r="F3" s="20"/>
+      <c r="C3" s="15"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="16"/>
     </row>
     <row r="4" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="12" t="s">
+      <c r="C4" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="12" t="s">
+      <c r="D4" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="12" t="s">
+      <c r="E4" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="F4" s="13" t="s">
+      <c r="F4" s="8" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B5" s="21">
+      <c r="B5" s="13">
         <v>1</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="C5" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="D5" s="9" t="s">
+      <c r="D5" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="E5" s="9" t="s">
+      <c r="E5" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="F5" s="10">
+      <c r="F5" s="5">
         <v>450</v>
       </c>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B6" s="14">
+      <c r="B6" s="9">
         <v>2</v>
       </c>
       <c r="C6" s="2" t="s">
@@ -924,12 +992,12 @@
       <c r="E6" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="F6" s="4">
+      <c r="F6" s="3">
         <v>400</v>
       </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B7" s="14">
+      <c r="B7" s="9">
         <v>3</v>
       </c>
       <c r="C7" s="2" t="s">
@@ -941,12 +1009,12 @@
       <c r="E7" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="F7" s="4">
+      <c r="F7" s="3">
         <v>350</v>
       </c>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B8" s="14">
+      <c r="B8" s="9">
         <v>4</v>
       </c>
       <c r="C8" s="2" t="s">
@@ -958,12 +1026,12 @@
       <c r="E8" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="F8" s="4">
+      <c r="F8" s="3">
         <v>300</v>
       </c>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B9" s="14">
+      <c r="B9" s="9">
         <v>5</v>
       </c>
       <c r="C9" s="2" t="s">
@@ -975,12 +1043,12 @@
       <c r="E9" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="F9" s="4">
+      <c r="F9" s="3">
         <v>250</v>
       </c>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B10" s="14">
+      <c r="B10" s="9">
         <v>6</v>
       </c>
       <c r="C10" s="2" t="s">
@@ -992,12 +1060,12 @@
       <c r="E10" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="F10" s="4">
+      <c r="F10" s="3">
         <v>200</v>
       </c>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B11" s="14">
+      <c r="B11" s="9">
         <v>7</v>
       </c>
       <c r="C11" s="2" t="s">
@@ -1009,12 +1077,12 @@
       <c r="E11" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="F11" s="4">
+      <c r="F11" s="3">
         <v>150</v>
       </c>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B12" s="14">
+      <c r="B12" s="9">
         <v>8</v>
       </c>
       <c r="C12" s="2" t="s">
@@ -1026,12 +1094,12 @@
       <c r="E12" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="F12" s="4">
+      <c r="F12" s="3">
         <v>100</v>
       </c>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B13" s="14">
+      <c r="B13" s="9">
         <v>9</v>
       </c>
       <c r="C13" s="2" t="s">
@@ -1043,66 +1111,66 @@
       <c r="E13" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="F13" s="4">
+      <c r="F13" s="3">
         <v>50</v>
       </c>
     </row>
     <row r="14" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B14" s="15">
+      <c r="B14" s="10">
         <v>10</v>
       </c>
-      <c r="C14" s="16" t="s">
+      <c r="C14" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="D14" s="16" t="s">
+      <c r="D14" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="E14" s="16" t="s">
+      <c r="E14" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="F14" s="17">
+      <c r="F14" s="12">
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="16" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B16" s="18" t="s">
+      <c r="B16" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="C16" s="19"/>
-      <c r="D16" s="19"/>
-      <c r="E16" s="20"/>
+      <c r="C16" s="15"/>
+      <c r="D16" s="15"/>
+      <c r="E16" s="16"/>
     </row>
     <row r="17" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B17" s="11" t="s">
+      <c r="B17" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C17" s="12" t="s">
+      <c r="C17" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="D17" s="12" t="s">
+      <c r="D17" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="E17" s="13" t="s">
+      <c r="E17" s="8" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B18" s="21">
+      <c r="B18" s="13">
         <v>1</v>
       </c>
-      <c r="C18" s="9" t="s">
+      <c r="C18" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="D18" s="9" t="s">
+      <c r="D18" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="E18" s="10" t="s">
+      <c r="E18" s="5" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B19" s="14">
+      <c r="B19" s="9">
         <v>2</v>
       </c>
       <c r="C19" s="2" t="s">
@@ -1111,12 +1179,12 @@
       <c r="D19" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="E19" s="4" t="s">
+      <c r="E19" s="3" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B20" s="14">
+      <c r="B20" s="9">
         <v>3</v>
       </c>
       <c r="C20" s="2" t="s">
@@ -1125,12 +1193,12 @@
       <c r="D20" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E20" s="4" t="s">
+      <c r="E20" s="3" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B21" s="14">
+      <c r="B21" s="9">
         <v>4</v>
       </c>
       <c r="C21" s="2" t="s">
@@ -1139,12 +1207,12 @@
       <c r="D21" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="E21" s="4" t="s">
+      <c r="E21" s="3" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B22" s="14">
+      <c r="B22" s="9">
         <v>5</v>
       </c>
       <c r="C22" s="2" t="s">
@@ -1153,12 +1221,12 @@
       <c r="D22" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="E22" s="4" t="s">
+      <c r="E22" s="3" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B23" s="14">
+      <c r="B23" s="9">
         <v>6</v>
       </c>
       <c r="C23" s="2" t="s">
@@ -1167,12 +1235,12 @@
       <c r="D23" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="E23" s="4" t="s">
+      <c r="E23" s="3" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B24" s="14">
+      <c r="B24" s="9">
         <v>7</v>
       </c>
       <c r="C24" s="2" t="s">
@@ -1181,12 +1249,12 @@
       <c r="D24" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="E24" s="4" t="s">
+      <c r="E24" s="3" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B25" s="14">
+      <c r="B25" s="9">
         <v>8</v>
       </c>
       <c r="C25" s="2" t="s">
@@ -1195,12 +1263,12 @@
       <c r="D25" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="E25" s="4" t="s">
+      <c r="E25" s="3" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="26" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B26" s="14">
+      <c r="B26" s="9">
         <v>9</v>
       </c>
       <c r="C26" s="2" t="s">
@@ -1209,21 +1277,21 @@
       <c r="D26" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E26" s="4" t="s">
+      <c r="E26" s="3" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="27" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B27" s="15">
+      <c r="B27" s="10">
         <v>10</v>
       </c>
-      <c r="C27" s="16" t="s">
+      <c r="C27" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="D27" s="16" t="s">
+      <c r="D27" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="E27" s="17" t="s">
+      <c r="E27" s="12" t="s">
         <v>47</v>
       </c>
     </row>

</xml_diff>